<commit_message>
add response tab and tested
</commit_message>
<xml_diff>
--- a/App_test_logs.xlsx
+++ b/App_test_logs.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://presagia-my.sharepoint.com/personal/xjia_telperian_com/Documents/Github/MetaToolEntry/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="8" documentId="13_ncr:1_{145FF1DB-C5BA-48E2-B1FC-61CED62AC782}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{3714E718-352D-4CE4-8CAE-30DE9C4285CE}"/>
+  <xr:revisionPtr revIDLastSave="12" documentId="13_ncr:1_{145FF1DB-C5BA-48E2-B1FC-61CED62AC782}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B686FDFB-1EAF-411E-8B4A-139A9F9078CC}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{F51B4368-EE33-4982-BF40-B1D646A43378}"/>
+    <workbookView xWindow="-93" yWindow="-93" windowWidth="25786" windowHeight="13866" xr2:uid="{F51B4368-EE33-4982-BF40-B1D646A43378}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="435" uniqueCount="178">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="437" uniqueCount="180">
   <si>
     <t>ID</t>
   </si>
@@ -616,6 +616,12 @@
   </si>
   <si>
     <t>1. no reponce</t>
+  </si>
+  <si>
+    <t>if RECIST save currectly</t>
+  </si>
+  <si>
+    <t>if response save currectly</t>
   </si>
 </sst>
 </file>
@@ -1038,28 +1044,28 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{555FF2D0-C6BF-430A-BA33-8F0900951C88}">
-  <dimension ref="A1:N80"/>
+  <dimension ref="A1:N82"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A72" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I74" sqref="I74"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A57" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="H81" sqref="H81"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
   <cols>
-    <col min="3" max="3" width="6.6328125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.90625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="25.26953125" style="2" customWidth="1"/>
+    <col min="3" max="3" width="6.64453125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.87890625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="25.29296875" style="2" customWidth="1"/>
     <col min="6" max="6" width="30" style="2" customWidth="1"/>
-    <col min="7" max="7" width="11.54296875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="35.26953125" style="2" customWidth="1"/>
-    <col min="9" max="9" width="44.81640625" style="2" customWidth="1"/>
-    <col min="10" max="10" width="16.81640625" customWidth="1"/>
-    <col min="11" max="12" width="9.90625" customWidth="1"/>
-    <col min="13" max="14" width="9.26953125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.52734375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="35.29296875" style="2" customWidth="1"/>
+    <col min="9" max="9" width="44.8203125" style="2" customWidth="1"/>
+    <col min="10" max="10" width="16.8203125" customWidth="1"/>
+    <col min="11" max="12" width="9.87890625" customWidth="1"/>
+    <col min="13" max="14" width="9.29296875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.5">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1100,7 +1106,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:13" s="5" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:13" s="5" customFormat="1" x14ac:dyDescent="0.5">
       <c r="B2" s="5">
         <v>1.1000000000000001</v>
       </c>
@@ -1132,7 +1138,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="3" spans="1:13" s="5" customFormat="1" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:13" s="5" customFormat="1" ht="43" x14ac:dyDescent="0.5">
       <c r="B3" s="5">
         <v>1.2</v>
       </c>
@@ -1164,7 +1170,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="4" spans="1:13" s="5" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:13" s="5" customFormat="1" x14ac:dyDescent="0.5">
       <c r="B4" s="5">
         <v>1.3</v>
       </c>
@@ -1196,7 +1202,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="5" spans="1:13" s="5" customFormat="1" ht="29" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:13" s="5" customFormat="1" ht="28.7" x14ac:dyDescent="0.5">
       <c r="B5" s="5">
         <v>2.1</v>
       </c>
@@ -1228,7 +1234,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="6" spans="1:13" s="5" customFormat="1" ht="29" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:13" s="5" customFormat="1" ht="28.7" x14ac:dyDescent="0.5">
       <c r="B6" s="5">
         <v>2.2000000000000002</v>
       </c>
@@ -1260,7 +1266,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="7" spans="1:13" s="5" customFormat="1" ht="29" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:13" s="5" customFormat="1" ht="28.7" x14ac:dyDescent="0.5">
       <c r="B7" s="5">
         <v>2.2999999999999998</v>
       </c>
@@ -1292,7 +1298,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="8" spans="1:13" s="5" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:13" s="5" customFormat="1" x14ac:dyDescent="0.5">
       <c r="B8" s="5">
         <v>2.4</v>
       </c>
@@ -1318,7 +1324,7 @@
       <c r="K8"/>
       <c r="L8"/>
     </row>
-    <row r="9" spans="1:13" s="5" customFormat="1" ht="29" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:13" s="5" customFormat="1" ht="28.7" x14ac:dyDescent="0.5">
       <c r="B9" s="5">
         <v>3.1</v>
       </c>
@@ -1350,7 +1356,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="10" spans="1:13" s="7" customFormat="1" ht="29" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:13" s="7" customFormat="1" ht="28.7" x14ac:dyDescent="0.5">
       <c r="B10" s="7" t="s">
         <v>65</v>
       </c>
@@ -1380,7 +1386,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="11" spans="1:13" s="7" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:13" s="7" customFormat="1" x14ac:dyDescent="0.5">
       <c r="B11" s="7" t="s">
         <v>119</v>
       </c>
@@ -1398,7 +1404,7 @@
       <c r="K11"/>
       <c r="L11"/>
     </row>
-    <row r="12" spans="1:13" s="9" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:13" s="9" customFormat="1" x14ac:dyDescent="0.5">
       <c r="E12" s="10"/>
       <c r="F12" s="10"/>
       <c r="H12" s="10"/>
@@ -1407,7 +1413,7 @@
       <c r="K12" s="11"/>
       <c r="L12" s="11"/>
     </row>
-    <row r="13" spans="1:13" s="5" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:13" s="5" customFormat="1" x14ac:dyDescent="0.5">
       <c r="B13" s="5">
         <v>11</v>
       </c>
@@ -1439,7 +1445,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="14" spans="1:13" s="5" customFormat="1" ht="29" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:13" s="5" customFormat="1" ht="28.7" x14ac:dyDescent="0.5">
       <c r="B14" s="5">
         <v>12.1</v>
       </c>
@@ -1471,7 +1477,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="15" spans="1:13" s="5" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:13" s="5" customFormat="1" x14ac:dyDescent="0.5">
       <c r="B15" s="5">
         <v>12.2</v>
       </c>
@@ -1503,7 +1509,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="16" spans="1:13" s="5" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:13" s="5" customFormat="1" x14ac:dyDescent="0.5">
       <c r="B16" s="5">
         <v>12.3</v>
       </c>
@@ -1535,7 +1541,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="17" spans="2:14" s="5" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="17" spans="2:14" s="5" customFormat="1" x14ac:dyDescent="0.5">
       <c r="B17" s="5">
         <v>12.4</v>
       </c>
@@ -1567,7 +1573,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="18" spans="2:14" s="5" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="18" spans="2:14" s="5" customFormat="1" x14ac:dyDescent="0.5">
       <c r="B18" s="5">
         <v>13</v>
       </c>
@@ -1599,7 +1605,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="19" spans="2:14" s="7" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="19" spans="2:14" s="7" customFormat="1" x14ac:dyDescent="0.5">
       <c r="B19" s="7" t="s">
         <v>121</v>
       </c>
@@ -1617,13 +1623,13 @@
       <c r="K19"/>
       <c r="L19"/>
     </row>
-    <row r="20" spans="2:14" s="9" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="20" spans="2:14" s="9" customFormat="1" x14ac:dyDescent="0.5">
       <c r="E20" s="10"/>
       <c r="F20" s="10"/>
       <c r="H20" s="10"/>
       <c r="I20" s="10"/>
     </row>
-    <row r="21" spans="2:14" s="15" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="21" spans="2:14" s="15" customFormat="1" x14ac:dyDescent="0.5">
       <c r="B21" s="16" t="s">
         <v>122</v>
       </c>
@@ -1638,7 +1644,7 @@
       <c r="H21" s="18"/>
       <c r="I21" s="18"/>
     </row>
-    <row r="22" spans="2:14" x14ac:dyDescent="0.35">
+    <row r="22" spans="2:14" x14ac:dyDescent="0.5">
       <c r="B22">
         <v>21.1</v>
       </c>
@@ -1671,7 +1677,7 @@
       </c>
       <c r="N22" s="4"/>
     </row>
-    <row r="23" spans="2:14" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="23" spans="2:14" ht="43" x14ac:dyDescent="0.5">
       <c r="B23">
         <v>21.2</v>
       </c>
@@ -1704,7 +1710,7 @@
       </c>
       <c r="N23" s="4"/>
     </row>
-    <row r="24" spans="2:14" ht="16" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="24" spans="2:14" ht="16" customHeight="1" x14ac:dyDescent="0.5">
       <c r="B24">
         <v>21.3</v>
       </c>
@@ -1737,7 +1743,7 @@
       </c>
       <c r="N24" s="4"/>
     </row>
-    <row r="25" spans="2:14" s="12" customFormat="1" ht="28.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="25" spans="2:14" s="12" customFormat="1" ht="28.75" customHeight="1" x14ac:dyDescent="0.5">
       <c r="B25" s="12">
         <v>22.1</v>
       </c>
@@ -1761,7 +1767,7 @@
       </c>
       <c r="N25" s="14"/>
     </row>
-    <row r="26" spans="2:14" s="12" customFormat="1" ht="62" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="26" spans="2:14" s="12" customFormat="1" ht="62" customHeight="1" x14ac:dyDescent="0.5">
       <c r="B26" s="12">
         <v>22.2</v>
       </c>
@@ -1785,7 +1791,7 @@
       </c>
       <c r="N26" s="14"/>
     </row>
-    <row r="27" spans="2:14" s="12" customFormat="1" ht="33" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="27" spans="2:14" s="12" customFormat="1" ht="33" customHeight="1" x14ac:dyDescent="0.5">
       <c r="B27" s="12">
         <v>22.3</v>
       </c>
@@ -1809,7 +1815,7 @@
       </c>
       <c r="N27" s="14"/>
     </row>
-    <row r="28" spans="2:14" s="12" customFormat="1" ht="67.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="28" spans="2:14" s="12" customFormat="1" ht="67.75" customHeight="1" x14ac:dyDescent="0.5">
       <c r="B28" s="12">
         <v>22.4</v>
       </c>
@@ -1833,7 +1839,7 @@
       </c>
       <c r="N28" s="14"/>
     </row>
-    <row r="29" spans="2:14" s="12" customFormat="1" ht="31.4" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="29" spans="2:14" s="12" customFormat="1" ht="31.45" customHeight="1" x14ac:dyDescent="0.5">
       <c r="B29" s="12">
         <v>22.5</v>
       </c>
@@ -1857,7 +1863,7 @@
       </c>
       <c r="N29" s="14"/>
     </row>
-    <row r="30" spans="2:14" s="12" customFormat="1" ht="57.4" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="30" spans="2:14" s="12" customFormat="1" ht="57.45" customHeight="1" x14ac:dyDescent="0.5">
       <c r="B30" s="12">
         <v>22.6</v>
       </c>
@@ -1881,7 +1887,7 @@
       </c>
       <c r="N30" s="14"/>
     </row>
-    <row r="31" spans="2:14" s="5" customFormat="1" ht="29" x14ac:dyDescent="0.35">
+    <row r="31" spans="2:14" s="5" customFormat="1" ht="28.7" x14ac:dyDescent="0.5">
       <c r="B31" s="5">
         <v>23.1</v>
       </c>
@@ -1913,7 +1919,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="32" spans="2:14" s="5" customFormat="1" ht="29" x14ac:dyDescent="0.35">
+    <row r="32" spans="2:14" s="5" customFormat="1" ht="28.7" x14ac:dyDescent="0.5">
       <c r="B32" s="5">
         <v>23.2</v>
       </c>
@@ -1945,7 +1951,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="33" spans="2:14" s="5" customFormat="1" ht="29" x14ac:dyDescent="0.35">
+    <row r="33" spans="2:14" s="5" customFormat="1" ht="28.7" x14ac:dyDescent="0.5">
       <c r="B33" s="5">
         <v>23.3</v>
       </c>
@@ -1977,7 +1983,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="34" spans="2:14" s="5" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="34" spans="2:14" s="5" customFormat="1" x14ac:dyDescent="0.5">
       <c r="B34" s="5">
         <v>23.4</v>
       </c>
@@ -2009,7 +2015,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="35" spans="2:14" ht="25.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="35" spans="2:14" ht="25.75" customHeight="1" x14ac:dyDescent="0.5">
       <c r="B35" s="5">
         <v>23.5</v>
       </c>
@@ -2042,7 +2048,7 @@
       </c>
       <c r="N35" s="4"/>
     </row>
-    <row r="36" spans="2:14" ht="49" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="36" spans="2:14" ht="49" customHeight="1" x14ac:dyDescent="0.5">
       <c r="B36" s="5">
         <v>23.6</v>
       </c>
@@ -2066,7 +2072,7 @@
       </c>
       <c r="N36" s="4"/>
     </row>
-    <row r="37" spans="2:14" ht="44.4" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="37" spans="2:14" ht="44.45" customHeight="1" x14ac:dyDescent="0.5">
       <c r="B37" s="5">
         <v>23.7</v>
       </c>
@@ -2090,15 +2096,15 @@
       </c>
       <c r="N37" s="4"/>
     </row>
-    <row r="38" spans="2:14" x14ac:dyDescent="0.35">
+    <row r="38" spans="2:14" x14ac:dyDescent="0.5">
       <c r="E38"/>
       <c r="N38" s="4"/>
     </row>
-    <row r="39" spans="2:14" x14ac:dyDescent="0.35">
+    <row r="39" spans="2:14" x14ac:dyDescent="0.5">
       <c r="E39"/>
       <c r="N39" s="4"/>
     </row>
-    <row r="40" spans="2:14" x14ac:dyDescent="0.35">
+    <row r="40" spans="2:14" x14ac:dyDescent="0.5">
       <c r="B40">
         <v>24.1</v>
       </c>
@@ -2122,7 +2128,7 @@
       </c>
       <c r="N40" s="4"/>
     </row>
-    <row r="41" spans="2:14" ht="72.5" x14ac:dyDescent="0.35">
+    <row r="41" spans="2:14" ht="71.7" x14ac:dyDescent="0.5">
       <c r="B41">
         <v>24.2</v>
       </c>
@@ -2143,7 +2149,7 @@
       </c>
       <c r="N41" s="4"/>
     </row>
-    <row r="42" spans="2:14" x14ac:dyDescent="0.35">
+    <row r="42" spans="2:14" x14ac:dyDescent="0.5">
       <c r="B42">
         <v>24.3</v>
       </c>
@@ -2164,7 +2170,7 @@
       </c>
       <c r="N42" s="4"/>
     </row>
-    <row r="43" spans="2:14" x14ac:dyDescent="0.35">
+    <row r="43" spans="2:14" x14ac:dyDescent="0.5">
       <c r="B43">
         <v>24.4</v>
       </c>
@@ -2185,7 +2191,7 @@
       </c>
       <c r="N43" s="4"/>
     </row>
-    <row r="44" spans="2:14" x14ac:dyDescent="0.35">
+    <row r="44" spans="2:14" x14ac:dyDescent="0.5">
       <c r="B44">
         <v>24.5</v>
       </c>
@@ -2206,14 +2212,14 @@
       </c>
       <c r="N44" s="4"/>
     </row>
-    <row r="45" spans="2:14" x14ac:dyDescent="0.35">
+    <row r="45" spans="2:14" x14ac:dyDescent="0.5">
       <c r="E45"/>
       <c r="G45" t="s">
         <v>14</v>
       </c>
       <c r="N45" s="4"/>
     </row>
-    <row r="46" spans="2:14" ht="29" x14ac:dyDescent="0.35">
+    <row r="46" spans="2:14" x14ac:dyDescent="0.5">
       <c r="B46">
         <v>25.1</v>
       </c>
@@ -2228,7 +2234,7 @@
       </c>
       <c r="N46" s="4"/>
     </row>
-    <row r="47" spans="2:14" ht="29" x14ac:dyDescent="0.35">
+    <row r="47" spans="2:14" ht="28.7" x14ac:dyDescent="0.5">
       <c r="B47">
         <v>25.2</v>
       </c>
@@ -2261,7 +2267,7 @@
       </c>
       <c r="N47" s="4"/>
     </row>
-    <row r="48" spans="2:14" ht="29" x14ac:dyDescent="0.35">
+    <row r="48" spans="2:14" ht="28.7" x14ac:dyDescent="0.5">
       <c r="E48" s="2" t="s">
         <v>94</v>
       </c>
@@ -2270,7 +2276,7 @@
       </c>
       <c r="N48" s="4"/>
     </row>
-    <row r="49" spans="2:14" ht="29" x14ac:dyDescent="0.35">
+    <row r="49" spans="2:14" x14ac:dyDescent="0.5">
       <c r="E49" s="2" t="s">
         <v>94</v>
       </c>
@@ -2279,7 +2285,7 @@
       </c>
       <c r="N49" s="4"/>
     </row>
-    <row r="50" spans="2:14" x14ac:dyDescent="0.35">
+    <row r="50" spans="2:14" x14ac:dyDescent="0.5">
       <c r="B50">
         <v>25.3</v>
       </c>
@@ -2302,7 +2308,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="51" spans="2:14" ht="29" x14ac:dyDescent="0.35">
+    <row r="51" spans="2:14" x14ac:dyDescent="0.5">
       <c r="D51" t="s">
         <v>6</v>
       </c>
@@ -2322,7 +2328,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="52" spans="2:14" ht="29" x14ac:dyDescent="0.35">
+    <row r="52" spans="2:14" x14ac:dyDescent="0.5">
       <c r="D52" t="s">
         <v>6</v>
       </c>
@@ -2342,7 +2348,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="53" spans="2:14" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="53" spans="2:14" ht="43" x14ac:dyDescent="0.5">
       <c r="D53" t="s">
         <v>6</v>
       </c>
@@ -2362,7 +2368,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="54" spans="2:14" ht="72.5" x14ac:dyDescent="0.35">
+    <row r="54" spans="2:14" ht="71.7" x14ac:dyDescent="0.5">
       <c r="D54" t="s">
         <v>6</v>
       </c>
@@ -2382,7 +2388,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="55" spans="2:14" ht="29" x14ac:dyDescent="0.35">
+    <row r="55" spans="2:14" ht="28.7" x14ac:dyDescent="0.5">
       <c r="D55" t="s">
         <v>6</v>
       </c>
@@ -2393,7 +2399,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="56" spans="2:14" ht="29" x14ac:dyDescent="0.35">
+    <row r="56" spans="2:14" ht="28.7" x14ac:dyDescent="0.5">
       <c r="D56" t="s">
         <v>6</v>
       </c>
@@ -2404,28 +2410,28 @@
         <v>167</v>
       </c>
     </row>
-    <row r="57" spans="2:14" x14ac:dyDescent="0.35">
+    <row r="57" spans="2:14" x14ac:dyDescent="0.5">
       <c r="D57" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="58" spans="2:14" x14ac:dyDescent="0.35">
+    <row r="58" spans="2:14" x14ac:dyDescent="0.5">
       <c r="D58" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="59" spans="2:14" x14ac:dyDescent="0.35">
+    <row r="59" spans="2:14" x14ac:dyDescent="0.5">
       <c r="D59" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="60" spans="2:14" s="11" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="60" spans="2:14" s="11" customFormat="1" x14ac:dyDescent="0.5">
       <c r="E60" s="19"/>
       <c r="F60" s="19"/>
       <c r="H60" s="19"/>
       <c r="I60" s="19"/>
     </row>
-    <row r="61" spans="2:14" ht="29" x14ac:dyDescent="0.35">
+    <row r="61" spans="2:14" ht="28.7" x14ac:dyDescent="0.5">
       <c r="B61">
         <v>31.1</v>
       </c>
@@ -2445,13 +2451,13 @@
         <v>134</v>
       </c>
     </row>
-    <row r="62" spans="2:14" s="11" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="62" spans="2:14" s="11" customFormat="1" x14ac:dyDescent="0.5">
       <c r="E62" s="19"/>
       <c r="F62" s="19"/>
       <c r="H62" s="19"/>
       <c r="I62" s="19"/>
     </row>
-    <row r="63" spans="2:14" ht="29" x14ac:dyDescent="0.35">
+    <row r="63" spans="2:14" ht="28.7" x14ac:dyDescent="0.5">
       <c r="B63">
         <v>41.1</v>
       </c>
@@ -2471,7 +2477,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="64" spans="2:14" x14ac:dyDescent="0.35">
+    <row r="64" spans="2:14" x14ac:dyDescent="0.5">
       <c r="D64" t="s">
         <v>129</v>
       </c>
@@ -2488,7 +2494,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="65" spans="2:9" ht="29" x14ac:dyDescent="0.35">
+    <row r="65" spans="2:9" ht="28.7" x14ac:dyDescent="0.5">
       <c r="D65" t="s">
         <v>129</v>
       </c>
@@ -2505,7 +2511,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="66" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="66" spans="2:9" x14ac:dyDescent="0.5">
       <c r="D66" t="s">
         <v>129</v>
       </c>
@@ -2519,7 +2525,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="67" spans="2:9" ht="29" x14ac:dyDescent="0.35">
+    <row r="67" spans="2:9" ht="28.7" x14ac:dyDescent="0.5">
       <c r="D67" t="s">
         <v>129</v>
       </c>
@@ -2536,7 +2542,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="68" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="68" spans="2:9" x14ac:dyDescent="0.5">
       <c r="D68" t="s">
         <v>129</v>
       </c>
@@ -2551,7 +2557,7 @@
       </c>
       <c r="H68" s="8"/>
     </row>
-    <row r="69" spans="2:9" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="69" spans="2:9" ht="43" x14ac:dyDescent="0.5">
       <c r="D69" t="s">
         <v>129</v>
       </c>
@@ -2568,7 +2574,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="70" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="70" spans="2:9" x14ac:dyDescent="0.5">
       <c r="D70" t="s">
         <v>129</v>
       </c>
@@ -2585,7 +2591,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="71" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="71" spans="2:9" x14ac:dyDescent="0.5">
       <c r="D71" t="s">
         <v>129</v>
       </c>
@@ -2602,7 +2608,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="72" spans="2:9" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="72" spans="2:9" ht="43" x14ac:dyDescent="0.5">
       <c r="D72" t="s">
         <v>129</v>
       </c>
@@ -2619,7 +2625,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="73" spans="2:9" ht="58" x14ac:dyDescent="0.35">
+    <row r="73" spans="2:9" ht="57.35" x14ac:dyDescent="0.5">
       <c r="D73" t="s">
         <v>129</v>
       </c>
@@ -2636,7 +2642,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="74" spans="2:9" ht="58" x14ac:dyDescent="0.35">
+    <row r="74" spans="2:9" ht="57.35" x14ac:dyDescent="0.5">
       <c r="D74" t="s">
         <v>129</v>
       </c>
@@ -2653,7 +2659,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="75" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="75" spans="2:9" x14ac:dyDescent="0.5">
       <c r="D75" t="s">
         <v>129</v>
       </c>
@@ -2670,13 +2676,13 @@
         <v>177</v>
       </c>
     </row>
-    <row r="77" spans="2:9" s="11" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="77" spans="2:9" s="11" customFormat="1" x14ac:dyDescent="0.5">
       <c r="E77" s="19"/>
       <c r="F77" s="19"/>
       <c r="H77" s="19"/>
       <c r="I77" s="19"/>
     </row>
-    <row r="78" spans="2:9" ht="29" x14ac:dyDescent="0.35">
+    <row r="78" spans="2:9" ht="28.7" x14ac:dyDescent="0.5">
       <c r="B78">
         <v>51.1</v>
       </c>
@@ -2699,12 +2705,12 @@
         <v>139</v>
       </c>
     </row>
-    <row r="79" spans="2:9" ht="29" x14ac:dyDescent="0.35">
+    <row r="79" spans="2:9" ht="28.7" x14ac:dyDescent="0.5">
       <c r="E79" s="2" t="s">
         <v>149</v>
       </c>
     </row>
-    <row r="80" spans="2:9" ht="29" x14ac:dyDescent="0.35">
+    <row r="80" spans="2:9" ht="28.7" x14ac:dyDescent="0.5">
       <c r="E80" s="2" t="s">
         <v>153</v>
       </c>
@@ -2716,6 +2722,16 @@
       </c>
       <c r="I80" s="2" t="s">
         <v>157</v>
+      </c>
+    </row>
+    <row r="81" spans="5:5" x14ac:dyDescent="0.5">
+      <c r="E81" s="2" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="82" spans="5:5" x14ac:dyDescent="0.5">
+      <c r="E82" s="2" t="s">
+        <v>179</v>
       </c>
     </row>
   </sheetData>

</xml_diff>